<commit_message>
osm - bip - orígenes
</commit_message>
<xml_diff>
--- a/origenes/Modelo Mapas OSM.xlsx
+++ b/origenes/Modelo Mapas OSM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/Escritorio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="345" documentId="13_ncr:1_{294123FD-9322-407A-B4D2-8C6293AB9611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87DD322F-D539-4260-A5CE-884BE346F277}"/>
+  <xr:revisionPtr revIDLastSave="346" documentId="13_ncr:1_{294123FD-9322-407A-B4D2-8C6293AB9611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE3C9611-D7B3-4613-AEB9-71D16325911E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{235109B0-F166-4A15-AA6B-2FE3B1F3995A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{235109B0-F166-4A15-AA6B-2FE3B1F3995A}"/>
   </bookViews>
   <sheets>
     <sheet name="Capas" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="25" r:id="rId9"/>
+    <pivotCache cacheId="32" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4480" uniqueCount="1327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4480" uniqueCount="1338">
   <si>
     <t>Capa</t>
   </si>
@@ -4066,6 +4066,39 @@
   </si>
   <si>
     <t>osm</t>
+  </si>
+  <si>
+    <t>natural_cumbre_de_montania</t>
+  </si>
+  <si>
+    <t>punto_de_interes_banio_pol</t>
+  </si>
+  <si>
+    <t>carreteras-muy_pequenias_pista_pol</t>
+  </si>
+  <si>
+    <t>punto_de_interes_banio</t>
+  </si>
+  <si>
+    <t>carreteras-muy_pequenias_pista</t>
+  </si>
+  <si>
+    <t>punto_de_interes_en_agua_puerto_pequenio_pol</t>
+  </si>
+  <si>
+    <t>trafico_senial_de_cruce</t>
+  </si>
+  <si>
+    <t>trafico_seniales_de_trafico</t>
+  </si>
+  <si>
+    <t>trafico_senial_de_alto</t>
+  </si>
+  <si>
+    <t>trafico_pequenia_rotonda</t>
+  </si>
+  <si>
+    <t>punto_de_interes_en_agua_puerto_pequenio</t>
   </si>
 </sst>
 </file>
@@ -4525,70 +4558,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="10"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -4685,6 +4654,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4814,6 +4803,50 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -8011,7 +8044,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B551A705-4F60-452F-BD65-EB017D0FFC91}" name="TablaDinámica1" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B551A705-4F60-452F-BD65-EB017D0FFC91}" name="TablaDinámica1" cacheId="32" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:C23" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="10">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -8693,9 +8726,9 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{3DCCD367-4176-4B1B-9DB1-7E15C5AB3C2E}" name="idcapa" dataDxfId="44"/>
     <tableColumn id="2" xr3:uid="{84365576-6006-4249-8C10-3C939914AB46}" name="Capa" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{23CB737A-7056-44F6-A537-CEB5ED7BC8A4}" name="Tipo" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{77A06ECF-D67C-454F-B0CE-327D202410E8}" name="url_ícono" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{041AD1F6-23D8-4ACA-92DC-196A5ACE0392}" name="url" dataDxfId="26">
+    <tableColumn id="3" xr3:uid="{23CB737A-7056-44F6-A537-CEB5ED7BC8A4}" name="Tipo" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{77A06ECF-D67C-454F-B0CE-327D202410E8}" name="url_ícono" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{041AD1F6-23D8-4ACA-92DC-196A5ACE0392}" name="url" dataDxfId="40">
       <calculatedColumnFormula>+"https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/"&amp;Capas[[#This Row],[url_ícono]]&amp;"/"&amp;Capas[[#This Row],[Capa]]&amp;"/?CUT_COM=00000.json"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8704,21 +8737,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B860159C-4E5B-4F1C-AD34-ACA1A658D8AB}" name="BD_Capas" displayName="BD_Capas" ref="A9:J209" totalsRowShown="0" headerRowDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B860159C-4E5B-4F1C-AD34-ACA1A658D8AB}" name="BD_Capas" displayName="BD_Capas" ref="A9:J209" totalsRowShown="0" headerRowDxfId="38">
   <autoFilter ref="A9:J209" xr:uid="{B860159C-4E5B-4F1C-AD34-ACA1A658D8AB}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{75A8A884-1D65-4E5E-B8C8-77E85AB66F2B}" name="idcapa" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{75A8A884-1D65-4E5E-B8C8-77E85AB66F2B}" name="idcapa" dataDxfId="37"/>
     <tableColumn id="2" xr3:uid="{2A8A9E62-F4FC-4E3B-B1C9-6BF40AA34453}" name="Capa">
       <calculatedColumnFormula>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{4562EDE5-8829-40E2-976E-2AE44EC10CA3}" name="idpropiedad"/>
     <tableColumn id="4" xr3:uid="{32385EA8-BAB7-4928-A031-A960AD89E53A}" name="Propiedad"/>
-    <tableColumn id="5" xr3:uid="{035EE145-9D77-4858-89B3-36E33AB1DD42}" name="popup_0_1" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{A9A0E11B-B8EA-4D4C-9546-EA4565E015BB}" name="descripcion_pop-up" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{5F6D8D2E-E38C-46CC-8F2C-5ED1D580678F}" name="posicion_popup" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{035EE145-9D77-4858-89B3-36E33AB1DD42}" name="popup_0_1" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{A9A0E11B-B8EA-4D4C-9546-EA4565E015BB}" name="descripcion_pop-up" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{5F6D8D2E-E38C-46CC-8F2C-5ED1D580678F}" name="posicion_popup" dataDxfId="34"/>
     <tableColumn id="8" xr3:uid="{8B5DC378-B7F9-4E3D-AC39-A4AF81250C0B}" name="descripcion_capa"/>
-    <tableColumn id="9" xr3:uid="{5C03E193-7980-49E1-894D-9DEECE0C9DBE}" name="clase" dataDxfId="37"/>
-    <tableColumn id="10" xr3:uid="{92421CFC-4A75-4D76-9B47-B3E7C2151B6C}" name="posición_capa" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{5C03E193-7980-49E1-894D-9DEECE0C9DBE}" name="clase" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{92421CFC-4A75-4D76-9B47-B3E7C2151B6C}" name="posición_capa" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8734,25 +8767,25 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{9D7FBDA9-0788-4563-AA35-00082D95202E}" name="Clase" dataDxfId="35">
+    <tableColumn id="1" xr3:uid="{9D7FBDA9-0788-4563-AA35-00082D95202E}" name="Clase" dataDxfId="29">
       <calculatedColumnFormula>+A9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{83BA5E88-8850-4C0E-B07A-7893981D4057}" name="Descripción Capa" dataDxfId="34">
+    <tableColumn id="7" xr3:uid="{83BA5E88-8850-4C0E-B07A-7893981D4057}" name="Descripción Capa" dataDxfId="28">
       <calculatedColumnFormula>+IFERROR(VLOOKUP(BD_Detalles[[#This Row],[Clase]],'Resumen Capas'!$A$4:$B$1048576,2,0),"COMPLETAR")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{487EB0A1-9443-44A7-BFE7-ACE9A32F49FF}" name="Propiedad" dataDxfId="33">
+    <tableColumn id="2" xr3:uid="{487EB0A1-9443-44A7-BFE7-ACE9A32F49FF}" name="Propiedad" dataDxfId="27">
       <calculatedColumnFormula>+IFERROR(IF(RIGHT(BD_Detalles[[#This Row],[Clase]],1)="0","",VLOOKUP(BD_Detalles[[#This Row],[Clase]],'Resumen Capas'!$A$4:$C$1048576,3,0)),"COMPLETAR")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{98AF95EE-6F82-4642-89B4-4DB0AA49AEEB}" name="Variable" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{98AF95EE-6F82-4642-89B4-4DB0AA49AEEB}" name="Variable" dataDxfId="26"/>
     <tableColumn id="4" xr3:uid="{5414C827-224B-4470-A9E1-6A29EF6EA250}" name="Color"/>
-    <tableColumn id="5" xr3:uid="{FA622BA5-65BA-42EE-91CA-9F9E3510C671}" name="titulo_leyenda" dataDxfId="31">
+    <tableColumn id="5" xr3:uid="{FA622BA5-65BA-42EE-91CA-9F9E3510C671}" name="titulo_leyenda" dataDxfId="25">
       <calculatedColumnFormula>+IFERROR(VLOOKUP(BD_Detalles[[#This Row],[Clase]],'Resumen Capas'!$A$4:$C$1048576,2,0),"COMPLETAR")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{32C0C72A-08F6-4017-AEC8-0A0B019C2C03}" name="url_icono" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{02FCDEF8-A182-4154-ACFD-C31BD15BAC9D}" name="idcapa" dataDxfId="29">
+    <tableColumn id="6" xr3:uid="{32C0C72A-08F6-4017-AEC8-0A0B019C2C03}" name="url_icono" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{02FCDEF8-A182-4154-ACFD-C31BD15BAC9D}" name="idcapa" dataDxfId="23">
       <calculatedColumnFormula>+LEFT(BD_Detalles[[#This Row],[Clase]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0DAE07AA-CA28-46ED-BED9-EDE4E800CFF8}" name="Tipo" dataDxfId="28">
+    <tableColumn id="9" xr3:uid="{0DAE07AA-CA28-46ED-BED9-EDE4E800CFF8}" name="Tipo" dataDxfId="22">
       <calculatedColumnFormula>+VLOOKUP(BD_Detalles[[#This Row],[idcapa]],Capas[[idcapa]:[Tipo]],3,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8768,21 +8801,21 @@
   </sortState>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{8DAF46F0-0587-4791-BD3B-29C4950AC864}" uniqueName="1" name="idcapa" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{A5538333-8E57-48D9-8222-03DAA80989CB}" uniqueName="2" name="Capa" queryTableFieldId="2" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{A5538333-8E57-48D9-8222-03DAA80989CB}" uniqueName="2" name="Capa" queryTableFieldId="2" dataDxfId="21"/>
     <tableColumn id="3" xr3:uid="{42797560-E23E-4585-909F-D47B8BA464C8}" uniqueName="3" name="idpropiedad" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{39BB973A-AB48-4770-AA48-2EB263D61EC2}" uniqueName="4" name="Propiedad" queryTableFieldId="4" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{39BB973A-AB48-4770-AA48-2EB263D61EC2}" uniqueName="4" name="Propiedad" queryTableFieldId="4" dataDxfId="20"/>
     <tableColumn id="5" xr3:uid="{198F6B35-CBC8-430F-99DE-B71C75248DA3}" uniqueName="5" name="popup_0_1" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{C25F2E29-5148-4959-B8FE-CF7EE98E5DEB}" uniqueName="6" name="descripcion_pop-up" queryTableFieldId="6" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{C25F2E29-5148-4959-B8FE-CF7EE98E5DEB}" uniqueName="6" name="descripcion_pop-up" queryTableFieldId="6" dataDxfId="19"/>
     <tableColumn id="7" xr3:uid="{334857B2-053C-4714-8654-E075BF03F0A8}" uniqueName="7" name="posicion_popup" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{A9873B2C-1B46-4611-BD52-0A97C7D21EAF}" uniqueName="8" name="descripcion_capa" queryTableFieldId="8" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{32B2ED96-0DD6-4ADE-87AF-B7ED7A0534FB}" uniqueName="9" name="clase" queryTableFieldId="9" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{A9873B2C-1B46-4611-BD52-0A97C7D21EAF}" uniqueName="8" name="descripcion_capa" queryTableFieldId="8" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{32B2ED96-0DD6-4ADE-87AF-B7ED7A0534FB}" uniqueName="9" name="clase" queryTableFieldId="9" dataDxfId="17"/>
     <tableColumn id="10" xr3:uid="{B2FB5E95-FA88-487B-9206-B6E7F079B714}" uniqueName="10" name="posición_capa" queryTableFieldId="10"/>
-    <tableColumn id="11" xr3:uid="{FAC68029-648A-4EAF-8C51-25A7C5E3FE1B}" uniqueName="11" name="Tipo" queryTableFieldId="11" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{FAC68029-648A-4EAF-8C51-25A7C5E3FE1B}" uniqueName="11" name="Tipo" queryTableFieldId="11" dataDxfId="16"/>
     <tableColumn id="12" xr3:uid="{B8E893AA-11D2-44FF-AF68-A0D5684C28DD}" uniqueName="12" name="url_ícono" queryTableFieldId="12"/>
-    <tableColumn id="13" xr3:uid="{611A6746-F84D-452C-9BE0-C23E3A4E17F2}" uniqueName="13" name="Propiedad.1" queryTableFieldId="13" dataDxfId="13"/>
-    <tableColumn id="14" xr3:uid="{9A72167E-DB9E-46B1-86CA-052167332E56}" uniqueName="14" name="Variable" queryTableFieldId="14" dataDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{13A7D352-24E4-4AFB-BF87-998BE16B0301}" uniqueName="15" name="Color" queryTableFieldId="15" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{6D4578CA-37C4-4E3D-943B-65A36077567C}" uniqueName="16" name="titulo_leyenda" queryTableFieldId="16" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{611A6746-F84D-452C-9BE0-C23E3A4E17F2}" uniqueName="13" name="Propiedad.1" queryTableFieldId="13" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{9A72167E-DB9E-46B1-86CA-052167332E56}" uniqueName="14" name="Variable" queryTableFieldId="14" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{13A7D352-24E4-4AFB-BF87-998BE16B0301}" uniqueName="15" name="Color" queryTableFieldId="15" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{6D4578CA-37C4-4E3D-943B-65A36077567C}" uniqueName="16" name="titulo_leyenda" queryTableFieldId="16" dataDxfId="12"/>
     <tableColumn id="17" xr3:uid="{D5652FBA-BB6D-44CF-B852-53BA455D7DC1}" uniqueName="17" name="url_icono" queryTableFieldId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -8794,8 +8827,8 @@
   <autoFilter ref="A1:E411" xr:uid="{291D560E-9CA4-4BAC-995A-F0E03B82B6EA}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{1B08FD65-382E-435D-851C-83A7049E1E56}" uniqueName="1" name="idcapa" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{BC737893-4EE0-435A-B6B2-871993B29D43}" uniqueName="2" name="Capa" queryTableFieldId="2" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{4014DA1F-B84E-4528-B682-D095C29B7876}" uniqueName="3" name="Tipo" queryTableFieldId="3" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{BC737893-4EE0-435A-B6B2-871993B29D43}" uniqueName="2" name="Capa" queryTableFieldId="2" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{4014DA1F-B84E-4528-B682-D095C29B7876}" uniqueName="3" name="Tipo" queryTableFieldId="3" dataDxfId="10"/>
     <tableColumn id="4" xr3:uid="{27281E59-8A0B-448F-86F0-552D99C834C8}" uniqueName="4" name="url_ícono" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{A53714B3-3AD4-46C4-BF24-27D0226DF032}" uniqueName="5" name="url" queryTableFieldId="5"/>
   </tableColumns>
@@ -9142,9 +9175,9 @@
   </sheetPr>
   <dimension ref="A1:E411"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9311,7 +9344,7 @@
         <v>472</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>61</v>
+        <v>1327</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>254</v>
@@ -9322,7 +9355,7 @@
       </c>
       <c r="E9" s="12" t="str">
         <f>+"https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/"&amp;Capas[[#This Row],[url_ícono]]&amp;"/"&amp;Capas[[#This Row],[Capa]]&amp;"/?CUT_COM=00000.json"</f>
-        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/natural_cumbre_de_montaña/?CUT_COM=00000.json</v>
+        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/natural_cumbre_de_montania/?CUT_COM=00000.json</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -10831,7 +10864,7 @@
         <v>552</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>968</v>
+        <v>1328</v>
       </c>
       <c r="C89" s="16" t="s">
         <v>22</v>
@@ -10842,7 +10875,7 @@
       </c>
       <c r="E89" s="12" t="str">
         <f>+"https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/"&amp;Capas[[#This Row],[url_ícono]]&amp;"/"&amp;Capas[[#This Row],[Capa]]&amp;"/?CUT_COM=00000.json"</f>
-        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/punto_de_interes_baño_pol/?CUT_COM=00000.json</v>
+        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/punto_de_interes_banio_pol/?CUT_COM=00000.json</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -11724,7 +11757,7 @@
         <v>594</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>1015</v>
+        <v>1329</v>
       </c>
       <c r="C136" s="16" t="s">
         <v>22</v>
@@ -11735,7 +11768,7 @@
       </c>
       <c r="E136" s="12" t="str">
         <f>+"https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/"&amp;Capas[[#This Row],[url_ícono]]&amp;"/"&amp;Capas[[#This Row],[Capa]]&amp;"/?CUT_COM=00000.json"</f>
-        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/carreteras-muy_pequeñas_pista_pol/?CUT_COM=00000.json</v>
+        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/carreteras-muy_pequenias_pista_pol/?CUT_COM=00000.json</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -13149,7 +13182,7 @@
         <v>664</v>
       </c>
       <c r="B211" s="13" t="s">
-        <v>119</v>
+        <v>1330</v>
       </c>
       <c r="C211" s="16" t="s">
         <v>254</v>
@@ -13160,7 +13193,7 @@
       </c>
       <c r="E211" s="12" t="str">
         <f>+"https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/"&amp;Capas[[#This Row],[url_ícono]]&amp;"/"&amp;Capas[[#This Row],[Capa]]&amp;"/?CUT_COM=00000.json"</f>
-        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/punto_de_interes_baño/?CUT_COM=00000.json</v>
+        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/punto_de_interes_banio/?CUT_COM=00000.json</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
@@ -15030,7 +15063,7 @@
         <v>757</v>
       </c>
       <c r="B310" s="13" t="s">
-        <v>166</v>
+        <v>1331</v>
       </c>
       <c r="C310" s="16" t="s">
         <v>254</v>
@@ -15041,7 +15074,7 @@
       </c>
       <c r="E310" s="12" t="str">
         <f>+"https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/"&amp;Capas[[#This Row],[url_ícono]]&amp;"/"&amp;Capas[[#This Row],[Capa]]&amp;"/?CUT_COM=00000.json"</f>
-        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/carreteras-muy_pequeñas_pista/?CUT_COM=00000.json</v>
+        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/carreteras-muy_pequenias_pista/?CUT_COM=00000.json</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.3">
@@ -15315,7 +15348,7 @@
         <v>772</v>
       </c>
       <c r="B325" s="13" t="s">
-        <v>1015</v>
+        <v>1329</v>
       </c>
       <c r="C325" s="16" t="s">
         <v>22</v>
@@ -15326,7 +15359,7 @@
       </c>
       <c r="E325" s="12" t="str">
         <f>+"https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/"&amp;Capas[[#This Row],[url_ícono]]&amp;"/"&amp;Capas[[#This Row],[Capa]]&amp;"/?CUT_COM=00000.json"</f>
-        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/carreteras-muy_pequeñas_pista_pol/?CUT_COM=00000.json</v>
+        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/carreteras-muy_pequenias_pista_pol/?CUT_COM=00000.json</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.3">
@@ -15885,7 +15918,7 @@
         <v>801</v>
       </c>
       <c r="B355" s="13" t="s">
-        <v>1097</v>
+        <v>1332</v>
       </c>
       <c r="C355" s="16" t="s">
         <v>22</v>
@@ -15896,7 +15929,7 @@
       </c>
       <c r="E355" s="12" t="str">
         <f>+"https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/"&amp;Capas[[#This Row],[url_ícono]]&amp;"/"&amp;Capas[[#This Row],[Capa]]&amp;"/?CUT_COM=00000.json"</f>
-        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/punto_de_interes_en_agua_puerto_pequeño_pol/?CUT_COM=00000.json</v>
+        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/punto_de_interes_en_agua_puerto_pequenio_pol/?CUT_COM=00000.json</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.3">
@@ -16132,7 +16165,7 @@
         <v>814</v>
       </c>
       <c r="B368" s="13" t="s">
-        <v>233</v>
+        <v>1333</v>
       </c>
       <c r="C368" s="16" t="s">
         <v>254</v>
@@ -16143,7 +16176,7 @@
       </c>
       <c r="E368" s="12" t="str">
         <f>+"https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/"&amp;Capas[[#This Row],[url_ícono]]&amp;"/"&amp;Capas[[#This Row],[Capa]]&amp;"/?CUT_COM=00000.json"</f>
-        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/trafico_señal_de_cruce/?CUT_COM=00000.json</v>
+        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/trafico_senial_de_cruce/?CUT_COM=00000.json</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.3">
@@ -16151,7 +16184,7 @@
         <v>815</v>
       </c>
       <c r="B369" s="13" t="s">
-        <v>234</v>
+        <v>1334</v>
       </c>
       <c r="C369" s="16" t="s">
         <v>254</v>
@@ -16162,7 +16195,7 @@
       </c>
       <c r="E369" s="12" t="str">
         <f>+"https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/"&amp;Capas[[#This Row],[url_ícono]]&amp;"/"&amp;Capas[[#This Row],[Capa]]&amp;"/?CUT_COM=00000.json"</f>
-        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/trafico_señales_de_trafico/?CUT_COM=00000.json</v>
+        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/trafico_seniales_de_trafico/?CUT_COM=00000.json</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.3">
@@ -16227,7 +16260,7 @@
         <v>819</v>
       </c>
       <c r="B373" s="13" t="s">
-        <v>236</v>
+        <v>1335</v>
       </c>
       <c r="C373" s="16" t="s">
         <v>254</v>
@@ -16238,7 +16271,7 @@
       </c>
       <c r="E373" s="12" t="str">
         <f>+"https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/"&amp;Capas[[#This Row],[url_ícono]]&amp;"/"&amp;Capas[[#This Row],[Capa]]&amp;"/?CUT_COM=00000.json"</f>
-        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/trafico_señal_de_alto/?CUT_COM=00000.json</v>
+        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/trafico_senial_de_alto/?CUT_COM=00000.json</v>
       </c>
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.3">
@@ -16246,7 +16279,7 @@
         <v>820</v>
       </c>
       <c r="B374" s="13" t="s">
-        <v>237</v>
+        <v>1336</v>
       </c>
       <c r="C374" s="16" t="s">
         <v>254</v>
@@ -16257,7 +16290,7 @@
       </c>
       <c r="E374" s="12" t="str">
         <f>+"https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/"&amp;Capas[[#This Row],[url_ícono]]&amp;"/"&amp;Capas[[#This Row],[Capa]]&amp;"/?CUT_COM=00000.json"</f>
-        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/trafico_pequeña_rotonda/?CUT_COM=00000.json</v>
+        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/trafico_pequenia_rotonda/?CUT_COM=00000.json</v>
       </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.3">
@@ -16303,7 +16336,7 @@
         <v>823</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>224</v>
+        <v>1337</v>
       </c>
       <c r="C377" s="16" t="s">
         <v>254</v>
@@ -16314,7 +16347,7 @@
       </c>
       <c r="E377" s="12" t="str">
         <f>+"https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/"&amp;Capas[[#This Row],[url_ícono]]&amp;"/"&amp;Capas[[#This Row],[Capa]]&amp;"/?CUT_COM=00000.json"</f>
-        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/punto_de_interes_en_agua_puerto_pequeño/?CUT_COM=00000.json</v>
+        <v>https://raw.githubusercontent.com/Sud-Austral/mapa_insumos2/main/osm/punto_de_interes_en_agua_puerto_pequenio/?CUT_COM=00000.json</v>
       </c>
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.3">
@@ -20393,7 +20426,7 @@
       </c>
       <c r="B150" s="23" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C150" s="30">
         <v>1</v>
@@ -20429,7 +20462,7 @@
       </c>
       <c r="B151" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C151" s="4">
         <v>2</v>
@@ -20450,7 +20483,7 @@
       </c>
       <c r="B152" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C152" s="4">
         <v>3</v>
@@ -20471,7 +20504,7 @@
       </c>
       <c r="B153" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C153" s="4">
         <v>4</v>
@@ -20492,7 +20525,7 @@
       </c>
       <c r="B154" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C154" s="4">
         <v>5</v>
@@ -20528,7 +20561,7 @@
       </c>
       <c r="B155" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C155" s="4">
         <v>6</v>
@@ -20549,7 +20582,7 @@
       </c>
       <c r="B156" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C156" s="4">
         <v>7</v>
@@ -20570,7 +20603,7 @@
       </c>
       <c r="B157" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C157" s="4">
         <v>8</v>
@@ -20591,7 +20624,7 @@
       </c>
       <c r="B158" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C158" s="4">
         <v>9</v>
@@ -20618,7 +20651,7 @@
       </c>
       <c r="B159" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C159" s="4">
         <v>10</v>
@@ -20639,7 +20672,7 @@
       </c>
       <c r="B160" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C160" s="4">
         <v>11</v>
@@ -20666,7 +20699,7 @@
       </c>
       <c r="B161" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C161" s="4">
         <v>12</v>
@@ -20687,7 +20720,7 @@
       </c>
       <c r="B162" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C162" s="4">
         <v>13</v>
@@ -20714,7 +20747,7 @@
       </c>
       <c r="B163" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C163" s="4">
         <v>14</v>
@@ -20735,7 +20768,7 @@
       </c>
       <c r="B164" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C164" s="4">
         <v>15</v>
@@ -20756,7 +20789,7 @@
       </c>
       <c r="B165" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C165" s="4">
         <v>16</v>
@@ -20777,7 +20810,7 @@
       </c>
       <c r="B166" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C166" s="4">
         <v>17</v>
@@ -20804,7 +20837,7 @@
       </c>
       <c r="B167" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C167" s="4">
         <v>18</v>
@@ -20831,7 +20864,7 @@
       </c>
       <c r="B168" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C168" s="4">
         <v>19</v>
@@ -20852,7 +20885,7 @@
       </c>
       <c r="B169" t="str">
         <f>+VLOOKUP(BD_Capas[[#This Row],[idcapa]],Capas[],2,0)</f>
-        <v>natural_cumbre_de_montaña</v>
+        <v>natural_cumbre_de_montania</v>
       </c>
       <c r="C169" s="4">
         <v>20</v>
@@ -21825,7 +21858,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E10:E209">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22537,12 +22570,12 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B11:B29">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>"COMPLETAR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:C29">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>"COMPLETAR"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22575,7 +22608,7 @@
   </sheetPr>
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>